<commit_message>
change lpce and lrg to class
</commit_message>
<xml_diff>
--- a/input_sample/M18001288W_input_sample.xlsx
+++ b/input_sample/M18001288W_input_sample.xlsx
@@ -30,10 +30,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>en_with</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ex_width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -51,6 +47,10 @@
   </si>
   <si>
     <t>ex_temp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>en_width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,7 +385,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -400,25 +400,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change imple of wr_grn_cr_scalar and fix mistakes in crlc Crn(including vector)
</commit_message>
<xml_diff>
--- a/input_sample/M18001288W_input_sample.xlsx
+++ b/input_sample/M18001288W_input_sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16399" windowHeight="6749"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16404" windowHeight="6744"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,19 +408,19 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>